<commit_message>
GFORMS-2637 Add new CAVR stencils
</commit_message>
<xml_diff>
--- a/conf/resources/animation-tax-relief-template.xlsx
+++ b/conf/resources/animation-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9F50945-97FE-405C-99FF-FB388DF5F545}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83B4C96E-79FB-4111-9DF5-3844F56AE2B4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animation Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -2119,8 +2119,8 @@
   </sheetPr>
   <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2644,19 +2644,19 @@
         <v>0</v>
       </c>
       <c r="E25" s="71">
-        <f>MIN(E19,E22)</f>
+        <f t="shared" ref="E25:H25" si="2">MIN(E21,E24)</f>
         <v>0</v>
       </c>
       <c r="F25" s="71">
-        <f>MIN(F19,F22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="71">
-        <f>MIN(G19,G22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="71">
-        <f>MIN(H19,H22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -2678,15 +2678,15 @@
         <v>0</v>
       </c>
       <c r="F26" s="71">
-        <f t="shared" ref="F26:H26" si="2">E25</f>
+        <f t="shared" ref="F26:H26" si="3">E25</f>
         <v>0</v>
       </c>
       <c r="G26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I26" s="15"/>
@@ -2773,19 +2773,19 @@
         <v>0</v>
       </c>
       <c r="E29" s="69">
-        <f t="shared" ref="E29:H29" si="3">E23</f>
+        <f t="shared" ref="E29:H29" si="4">E23</f>
         <v>0</v>
       </c>
       <c r="F29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I29" s="78"/>
@@ -2836,15 +2836,15 @@
         <v>0</v>
       </c>
       <c r="F31" s="69">
-        <f t="shared" ref="F31:H31" si="4">F29-F30</f>
+        <f t="shared" ref="F31:H31" si="5">F29-F30</f>
         <v>0</v>
       </c>
       <c r="G31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I31" s="78" t="s">
@@ -2909,19 +2909,19 @@
         <v>0</v>
       </c>
       <c r="E34" s="69">
-        <f t="shared" ref="E34:H34" si="5">SUM(E32-E33)</f>
+        <f t="shared" ref="E34:H34" si="6">SUM(E32-E33)</f>
         <v>0</v>
       </c>
       <c r="F34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I34" s="78" t="s">
@@ -2942,19 +2942,19 @@
         <v>0</v>
       </c>
       <c r="E35" s="69">
-        <f t="shared" ref="E35:H35" si="6">E31+E34</f>
+        <f t="shared" ref="E35:H35" si="7">E31+E34</f>
         <v>0</v>
       </c>
       <c r="F35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I35" s="78" t="s">
@@ -2975,19 +2975,19 @@
         <v>0</v>
       </c>
       <c r="E36" s="69">
-        <f t="shared" ref="E36:H36" si="7">E21</f>
+        <f t="shared" ref="E36:H36" si="8">E21</f>
         <v>0</v>
       </c>
       <c r="F36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I36" s="78"/>
@@ -3034,19 +3034,19 @@
         <v>0</v>
       </c>
       <c r="E38" s="69">
-        <f t="shared" ref="E38:H38" si="8">E36-E37</f>
+        <f t="shared" ref="E38:H38" si="9">E36-E37</f>
         <v>0</v>
       </c>
       <c r="F38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I38" s="78" t="s">
@@ -3125,11 +3125,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="71">
-        <f t="shared" ref="G41:H41" si="9">F41+F43</f>
+        <f t="shared" ref="G41:H41" si="10">F41+F43</f>
         <v>0</v>
       </c>
       <c r="H41" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I41" s="15"/>
@@ -3268,7 +3268,7 @@
       <c r="I48" s="74"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LgNRJMVwmbf9AUV5MZGvWh4Pcoz9vY+mEaPcg8v02ag7r99fdwvULiHPqY4lCP/umhi/kjLIEjtq5K1KQaEkRA==" saltValue="fequuD5v29GojcR1aHgZtQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8v+F8aI0tEjTVWj0ZCtVOjjxvbAbf/iXpPoQtWHSQefC2NPjaniI9upjjjkFBrJjR02r6yppvHI9iXV7GXdjWw==" saltValue="HN8VgQqKe9GSmtkg9BfKLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="D2:I2"/>
@@ -3383,7 +3383,7 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
@@ -3902,17 +3902,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196d710fa02d7b8454006001c59ff208">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dd5f73807ecc01be09f0551dd16e5ff" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fb86a6bd64274b76f239f5430f3f160">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e5356646ac113cdb6f7e4fb15d9e89" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <xsd:import namespace="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <xsd:element name="properties">
@@ -3928,6 +3919,11 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3963,6 +3959,31 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4095,16 +4116,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DCC61D1-F8ED-4604-BFC3-95AECA0CBB00}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -4113,15 +4143,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8BBECC6-08E6-4D42-BCD4-A12DEFC85450}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4836C5AD-8FE8-4773-8ABB-8D6AAB6EA289}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4137,4 +4159,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-2637 Add new CAVR stencils (#2104)
</commit_message>
<xml_diff>
--- a/conf/resources/animation-tax-relief-template.xlsx
+++ b/conf/resources/animation-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9F50945-97FE-405C-99FF-FB388DF5F545}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83B4C96E-79FB-4111-9DF5-3844F56AE2B4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animation Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -2119,8 +2119,8 @@
   </sheetPr>
   <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2644,19 +2644,19 @@
         <v>0</v>
       </c>
       <c r="E25" s="71">
-        <f>MIN(E19,E22)</f>
+        <f t="shared" ref="E25:H25" si="2">MIN(E21,E24)</f>
         <v>0</v>
       </c>
       <c r="F25" s="71">
-        <f>MIN(F19,F22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="71">
-        <f>MIN(G19,G22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="71">
-        <f>MIN(H19,H22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -2678,15 +2678,15 @@
         <v>0</v>
       </c>
       <c r="F26" s="71">
-        <f t="shared" ref="F26:H26" si="2">E25</f>
+        <f t="shared" ref="F26:H26" si="3">E25</f>
         <v>0</v>
       </c>
       <c r="G26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I26" s="15"/>
@@ -2773,19 +2773,19 @@
         <v>0</v>
       </c>
       <c r="E29" s="69">
-        <f t="shared" ref="E29:H29" si="3">E23</f>
+        <f t="shared" ref="E29:H29" si="4">E23</f>
         <v>0</v>
       </c>
       <c r="F29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I29" s="78"/>
@@ -2836,15 +2836,15 @@
         <v>0</v>
       </c>
       <c r="F31" s="69">
-        <f t="shared" ref="F31:H31" si="4">F29-F30</f>
+        <f t="shared" ref="F31:H31" si="5">F29-F30</f>
         <v>0</v>
       </c>
       <c r="G31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I31" s="78" t="s">
@@ -2909,19 +2909,19 @@
         <v>0</v>
       </c>
       <c r="E34" s="69">
-        <f t="shared" ref="E34:H34" si="5">SUM(E32-E33)</f>
+        <f t="shared" ref="E34:H34" si="6">SUM(E32-E33)</f>
         <v>0</v>
       </c>
       <c r="F34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I34" s="78" t="s">
@@ -2942,19 +2942,19 @@
         <v>0</v>
       </c>
       <c r="E35" s="69">
-        <f t="shared" ref="E35:H35" si="6">E31+E34</f>
+        <f t="shared" ref="E35:H35" si="7">E31+E34</f>
         <v>0</v>
       </c>
       <c r="F35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I35" s="78" t="s">
@@ -2975,19 +2975,19 @@
         <v>0</v>
       </c>
       <c r="E36" s="69">
-        <f t="shared" ref="E36:H36" si="7">E21</f>
+        <f t="shared" ref="E36:H36" si="8">E21</f>
         <v>0</v>
       </c>
       <c r="F36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I36" s="78"/>
@@ -3034,19 +3034,19 @@
         <v>0</v>
       </c>
       <c r="E38" s="69">
-        <f t="shared" ref="E38:H38" si="8">E36-E37</f>
+        <f t="shared" ref="E38:H38" si="9">E36-E37</f>
         <v>0</v>
       </c>
       <c r="F38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I38" s="78" t="s">
@@ -3125,11 +3125,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="71">
-        <f t="shared" ref="G41:H41" si="9">F41+F43</f>
+        <f t="shared" ref="G41:H41" si="10">F41+F43</f>
         <v>0</v>
       </c>
       <c r="H41" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I41" s="15"/>
@@ -3268,7 +3268,7 @@
       <c r="I48" s="74"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LgNRJMVwmbf9AUV5MZGvWh4Pcoz9vY+mEaPcg8v02ag7r99fdwvULiHPqY4lCP/umhi/kjLIEjtq5K1KQaEkRA==" saltValue="fequuD5v29GojcR1aHgZtQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8v+F8aI0tEjTVWj0ZCtVOjjxvbAbf/iXpPoQtWHSQefC2NPjaniI9upjjjkFBrJjR02r6yppvHI9iXV7GXdjWw==" saltValue="HN8VgQqKe9GSmtkg9BfKLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="D2:I2"/>
@@ -3383,7 +3383,7 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
@@ -3902,17 +3902,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196d710fa02d7b8454006001c59ff208">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dd5f73807ecc01be09f0551dd16e5ff" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fb86a6bd64274b76f239f5430f3f160">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e5356646ac113cdb6f7e4fb15d9e89" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <xsd:import namespace="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <xsd:element name="properties">
@@ -3928,6 +3919,11 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3963,6 +3959,31 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4095,16 +4116,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DCC61D1-F8ED-4604-BFC3-95AECA0CBB00}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -4113,15 +4143,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8BBECC6-08E6-4D42-BCD4-A12DEFC85450}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4836C5AD-8FE8-4773-8ABB-8D6AAB6EA289}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4137,4 +4159,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GFORMS-2637 hard reset for patch
</commit_message>
<xml_diff>
--- a/conf/resources/animation-tax-relief-template.xlsx
+++ b/conf/resources/animation-tax-relief-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmrc.sharepoint.com/teams/GRP042118873/Creative Industries/Creatives Reform 2022/IT Project/Stencils/Existing reliefs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9F50945-97FE-405C-99FF-FB388DF5F545}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_E1F356FB086E12F67AF1FC24BBC6E33B7DFCDFC0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83B4C96E-79FB-4111-9DF5-3844F56AE2B4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animation Tax Relief Stencil" sheetId="2" r:id="rId1"/>
@@ -2119,8 +2119,8 @@
   </sheetPr>
   <dimension ref="A2:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2644,19 +2644,19 @@
         <v>0</v>
       </c>
       <c r="E25" s="71">
-        <f>MIN(E19,E22)</f>
+        <f t="shared" ref="E25:H25" si="2">MIN(E21,E24)</f>
         <v>0</v>
       </c>
       <c r="F25" s="71">
-        <f>MIN(F19,F22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G25" s="71">
-        <f>MIN(G19,G22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H25" s="71">
-        <f>MIN(H19,H22)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -2678,15 +2678,15 @@
         <v>0</v>
       </c>
       <c r="F26" s="71">
-        <f t="shared" ref="F26:H26" si="2">E25</f>
+        <f t="shared" ref="F26:H26" si="3">E25</f>
         <v>0</v>
       </c>
       <c r="G26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H26" s="71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I26" s="15"/>
@@ -2773,19 +2773,19 @@
         <v>0</v>
       </c>
       <c r="E29" s="69">
-        <f t="shared" ref="E29:H29" si="3">E23</f>
+        <f t="shared" ref="E29:H29" si="4">E23</f>
         <v>0</v>
       </c>
       <c r="F29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H29" s="69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I29" s="78"/>
@@ -2836,15 +2836,15 @@
         <v>0</v>
       </c>
       <c r="F31" s="69">
-        <f t="shared" ref="F31:H31" si="4">F29-F30</f>
+        <f t="shared" ref="F31:H31" si="5">F29-F30</f>
         <v>0</v>
       </c>
       <c r="G31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H31" s="69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I31" s="78" t="s">
@@ -2909,19 +2909,19 @@
         <v>0</v>
       </c>
       <c r="E34" s="69">
-        <f t="shared" ref="E34:H34" si="5">SUM(E32-E33)</f>
+        <f t="shared" ref="E34:H34" si="6">SUM(E32-E33)</f>
         <v>0</v>
       </c>
       <c r="F34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H34" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I34" s="78" t="s">
@@ -2942,19 +2942,19 @@
         <v>0</v>
       </c>
       <c r="E35" s="69">
-        <f t="shared" ref="E35:H35" si="6">E31+E34</f>
+        <f t="shared" ref="E35:H35" si="7">E31+E34</f>
         <v>0</v>
       </c>
       <c r="F35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H35" s="69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I35" s="78" t="s">
@@ -2975,19 +2975,19 @@
         <v>0</v>
       </c>
       <c r="E36" s="69">
-        <f t="shared" ref="E36:H36" si="7">E21</f>
+        <f t="shared" ref="E36:H36" si="8">E21</f>
         <v>0</v>
       </c>
       <c r="F36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H36" s="69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I36" s="78"/>
@@ -3034,19 +3034,19 @@
         <v>0</v>
       </c>
       <c r="E38" s="69">
-        <f t="shared" ref="E38:H38" si="8">E36-E37</f>
+        <f t="shared" ref="E38:H38" si="9">E36-E37</f>
         <v>0</v>
       </c>
       <c r="F38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H38" s="69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I38" s="78" t="s">
@@ -3125,11 +3125,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="71">
-        <f t="shared" ref="G41:H41" si="9">F41+F43</f>
+        <f t="shared" ref="G41:H41" si="10">F41+F43</f>
         <v>0</v>
       </c>
       <c r="H41" s="71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I41" s="15"/>
@@ -3268,7 +3268,7 @@
       <c r="I48" s="74"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LgNRJMVwmbf9AUV5MZGvWh4Pcoz9vY+mEaPcg8v02ag7r99fdwvULiHPqY4lCP/umhi/kjLIEjtq5K1KQaEkRA==" saltValue="fequuD5v29GojcR1aHgZtQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8v+F8aI0tEjTVWj0ZCtVOjjxvbAbf/iXpPoQtWHSQefC2NPjaniI9upjjjkFBrJjR02r6yppvHI9iXV7GXdjWw==" saltValue="HN8VgQqKe9GSmtkg9BfKLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="D2:I2"/>
@@ -3383,7 +3383,7 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
@@ -3902,17 +3902,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="196d710fa02d7b8454006001c59ff208">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2dd5f73807ecc01be09f0551dd16e5ff" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100350E8E2BB23E2A4AA4EA2615525F2B5A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fb86a6bd64274b76f239f5430f3f160">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e4bfe8b-ef84-4e47-853e-31313f64a53a" xmlns:ns3="7058508a-d375-4a1e-a567-7dd1bee321db" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e5356646ac113cdb6f7e4fb15d9e89" ns2:_="" ns3:_="">
     <xsd:import namespace="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <xsd:import namespace="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <xsd:element name="properties">
@@ -3928,6 +3919,11 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3963,6 +3959,31 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -4095,16 +4116,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DCC61D1-F8ED-4604-BFC3-95AECA0CBB00}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="2e4bfe8b-ef84-4e47-853e-31313f64a53a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="7058508a-d375-4a1e-a567-7dd1bee321db"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -4113,15 +4143,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8BBECC6-08E6-4D42-BCD4-A12DEFC85450}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4836C5AD-8FE8-4773-8ABB-8D6AAB6EA289}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -4137,4 +4159,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{547491D6-8660-47EB-8D96-4577B1508712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>